<commit_message>
update sample data and add mroe complex date path replacements
</commit_message>
<xml_diff>
--- a/sample_data/2024/Q3/file_one.xlsx
+++ b/sample_data/2024/Q3/file_one.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Desktop/File_checks/sample_data/2024/Q3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8B08C84-E9C0-7245-84F6-016C37ED8DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A9756D-D352-784E-93B3-B459E0B8980F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17380" xr2:uid="{67557609-4120-AA4F-9954-86F4213F8599}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t>a</t>
   </si>
@@ -56,10 +57,16 @@
     <t>total</t>
   </si>
   <si>
-    <t>X</t>
+    <t>X Type</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>Y Type</t>
+  </si>
+  <si>
+    <t>junk</t>
+  </si>
+  <si>
+    <t>unk</t>
   </si>
 </sst>
 </file>
@@ -75,12 +82,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,101 +446,923 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFDBD2D-C2C5-2F47-8892-D28CE2656078}">
-  <dimension ref="A6:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C6" s="1">
+        <v>45322</v>
+      </c>
+      <c r="D6" s="1">
         <v>45350</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>45382</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>45412</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>45443</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>45473</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>45504</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>45535</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>45565</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>45596</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>40</v>
+      </c>
+      <c r="K8">
+        <v>50</v>
+      </c>
+      <c r="L8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <f>D8</f>
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:L9" si="0">E8</f>
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>101</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>101</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f>SUM(C8:C12)</f>
+        <v>232</v>
+      </c>
+      <c r="D13">
+        <f>SUM(D8:D12)</f>
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:L13" si="1">SUM(E8:E12)</f>
+        <v>65</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>40</v>
+      </c>
+      <c r="K16">
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <f>D16</f>
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:L17" si="2">E16</f>
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C16:C18)</f>
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:L19" si="3">SUM(D16:D18)</f>
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB44E79-105E-B94F-8C33-77B81466A2FD}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C6" s="1">
+        <v>45322</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45350</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45382</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45412</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45443</v>
+      </c>
+      <c r="H6" s="1">
+        <v>45473</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45504</v>
+      </c>
+      <c r="J6" s="1">
+        <v>45535</v>
+      </c>
+      <c r="K6" s="1">
+        <v>45565</v>
+      </c>
+      <c r="L6" s="1">
+        <v>45596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>40</v>
+      </c>
+      <c r="K8" s="2">
+        <v>50</v>
+      </c>
+      <c r="L8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <f>D8</f>
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:L9" si="0">E8</f>
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>101</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>101</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f>SUM(C8:C12)</f>
+        <v>232</v>
+      </c>
+      <c r="D13">
+        <f>SUM(D8:D12)</f>
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:L13" si="1">SUM(E8:E12)</f>
+        <v>65</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>40</v>
+      </c>
+      <c r="K16" s="2">
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <f>D16</f>
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:L17" si="2">E16</f>
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C16:C18)</f>
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:L19" si="3">SUM(D16:D18)</f>
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>